<commit_message>
Ricomincio progetto in R, esempio di uso del pacchetto psych
</commit_message>
<xml_diff>
--- a/EsameEXCEL.xlsx
+++ b/EsameEXCEL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\tesi\marco_cordoni_sw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\tesi\tesiSWR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,44 +14,119 @@
   <sheets>
     <sheet name="EsameCSV" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Studente</t>
   </si>
   <si>
-    <t>Esercizio 1</t>
-  </si>
-  <si>
-    <t>Esercizio 2</t>
-  </si>
-  <si>
-    <t>Esercizio 3</t>
-  </si>
-  <si>
-    <t>Esercizio 4</t>
-  </si>
-  <si>
-    <t>Esercizio 5</t>
-  </si>
-  <si>
-    <t>Marco</t>
-  </si>
-  <si>
-    <t>Simone</t>
-  </si>
-  <si>
-    <t>Davide</t>
-  </si>
-  <si>
-    <t>Edoardo</t>
-  </si>
-  <si>
-    <t>Alex</t>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
+  <si>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
+  <si>
+    <t>S25</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>e3</t>
+  </si>
+  <si>
+    <t>e4</t>
+  </si>
+  <si>
+    <t>e5</t>
+  </si>
+  <si>
+    <t>e6</t>
+  </si>
+  <si>
+    <t>e7</t>
+  </si>
+  <si>
+    <t>e8</t>
+  </si>
+  <si>
+    <t>e9</t>
+  </si>
+  <si>
+    <t>e10</t>
   </si>
 </sst>
 </file>
@@ -892,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="V18" sqref="U18:V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,124 +978,914 @@
     <col min="2" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>